<commit_message>
fixed issue with hold_time not displaying
</commit_message>
<xml_diff>
--- a/db/data/Calisthenics Skills.xlsx
+++ b/db/data/Calisthenics Skills.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nkmatsumoto/code/nkmatsumoto/form_calisthenics_app/db/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14ABC48-2046-4B4C-A0F8-73CDC34BE1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8322CD29-1569-8542-B662-EC1361A786C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="940" windowWidth="27180" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -722,8 +722,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="m\-d"/>
-    <numFmt numFmtId="167" formatCode="hh:mm"/>
+    <numFmt numFmtId="164" formatCode="m\-d"/>
+    <numFmt numFmtId="165" formatCode="hh:mm"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -1054,7 +1054,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1140,7 +1140,7 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1161,18 +1161,18 @@
     <xf numFmtId="49" fontId="15" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1395,8 +1395,8 @@
   </sheetPr>
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="213" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScale="213" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -2942,7 +2942,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="12">
         <v>10</v>
       </c>
@@ -3210,11 +3210,11 @@
       <c r="F1" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="H1" s="53"/>
-      <c r="I1" s="58"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="55"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
@@ -3225,9 +3225,9 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="58"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
@@ -3244,11 +3244,11 @@
         <v>3</v>
       </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="57" t="s">
+      <c r="G3" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="H3" s="53"/>
-      <c r="I3" s="58"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="55"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">
@@ -3265,11 +3265,11 @@
         <v>0.10416666666666667</v>
       </c>
       <c r="F4" s="8"/>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="59" t="s">
         <v>130</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="58"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="55"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
@@ -3286,11 +3286,11 @@
         <v>3</v>
       </c>
       <c r="F5" s="9"/>
-      <c r="G5" s="54" t="s">
+      <c r="G5" s="56" t="s">
         <v>134</v>
       </c>
-      <c r="H5" s="55"/>
-      <c r="I5" s="56"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="58"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
@@ -3307,11 +3307,11 @@
         <v>3</v>
       </c>
       <c r="F6" s="3"/>
-      <c r="G6" s="57" t="s">
+      <c r="G6" s="59" t="s">
         <v>138</v>
       </c>
-      <c r="H6" s="53"/>
-      <c r="I6" s="58"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="55"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13" t="s">
@@ -3328,11 +3328,11 @@
         <v>2</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="57" t="s">
+      <c r="G7" s="59" t="s">
         <v>142</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="58"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="55"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13" t="s">
@@ -3349,11 +3349,11 @@
         <v>2</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="57" t="s">
+      <c r="G8" s="59" t="s">
         <v>146</v>
       </c>
-      <c r="H8" s="53"/>
-      <c r="I8" s="58"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="55"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="13" t="s">
@@ -3370,11 +3370,11 @@
         <v>6.25E-2</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="57" t="s">
+      <c r="G9" s="59" t="s">
         <v>150</v>
       </c>
-      <c r="H9" s="53"/>
-      <c r="I9" s="58"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="55"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="13" t="s">
@@ -3385,9 +3385,9 @@
       <c r="D10" s="16"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="58"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="16"/>
@@ -3396,9 +3396,9 @@
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="58"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="42" t="s">
@@ -3419,9 +3419,9 @@
       <c r="F12" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="G12" s="54"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="58"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13" t="s">
@@ -3432,9 +3432,9 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="58"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13" t="s">
@@ -3451,11 +3451,11 @@
         <v>0.10416666666666667</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="54" t="s">
+      <c r="G14" s="56" t="s">
         <v>154</v>
       </c>
-      <c r="H14" s="55"/>
-      <c r="I14" s="56"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="58"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13" t="s">
@@ -3472,11 +3472,11 @@
         <v>0.10416666666666667</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="57" t="s">
+      <c r="G15" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="H15" s="53"/>
-      <c r="I15" s="58"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="55"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13" t="s">
@@ -3493,11 +3493,11 @@
         <v>3</v>
       </c>
       <c r="F16" s="16"/>
-      <c r="G16" s="54" t="s">
+      <c r="G16" s="56" t="s">
         <v>159</v>
       </c>
-      <c r="H16" s="55"/>
-      <c r="I16" s="56"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="58"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13" t="s">
@@ -3514,9 +3514,9 @@
         <v>3</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="58"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="55"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="13" t="s">
@@ -3533,11 +3533,11 @@
         <v>2</v>
       </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="54" t="s">
+      <c r="G18" s="56" t="s">
         <v>165</v>
       </c>
-      <c r="H18" s="55"/>
-      <c r="I18" s="56"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="58"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="13" t="s">
@@ -3554,11 +3554,11 @@
         <v>2</v>
       </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="59" t="s">
+      <c r="G19" s="60" t="s">
         <v>169</v>
       </c>
-      <c r="H19" s="53"/>
-      <c r="I19" s="58"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="55"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13" t="s">
@@ -3575,11 +3575,11 @@
         <v>6.25E-2</v>
       </c>
       <c r="F20" s="3"/>
-      <c r="G20" s="59" t="s">
+      <c r="G20" s="60" t="s">
         <v>172</v>
       </c>
-      <c r="H20" s="53"/>
-      <c r="I20" s="58"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="55"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="13" t="s">
@@ -3590,9 +3590,9 @@
       <c r="D21" s="16"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="56"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="58"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
@@ -3601,9 +3601,9 @@
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="58"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="42" t="s">
@@ -3624,9 +3624,9 @@
       <c r="F23" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="G23" s="54"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="58"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="13" t="s">
@@ -3637,9 +3637,9 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="58"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="13" t="s">
@@ -3658,9 +3658,9 @@
         <v>3</v>
       </c>
       <c r="F25" s="16"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="58"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="13" t="s">
@@ -3679,9 +3679,9 @@
         <v>3</v>
       </c>
       <c r="F26" s="16"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="56"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="58"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="13" t="s">
@@ -3702,11 +3702,11 @@
       <c r="F27" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="G27" s="57" t="s">
+      <c r="G27" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="H27" s="53"/>
-      <c r="I27" s="58"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="55"/>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="13" t="s">
@@ -3725,11 +3725,11 @@
         <v>2</v>
       </c>
       <c r="F28" s="16"/>
-      <c r="G28" s="57" t="s">
+      <c r="G28" s="59" t="s">
         <v>185</v>
       </c>
-      <c r="H28" s="53"/>
-      <c r="I28" s="58"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="55"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="13" t="s">
@@ -3746,11 +3746,11 @@
         <v>0.10416666666666667</v>
       </c>
       <c r="F29" s="16"/>
-      <c r="G29" s="57" t="s">
+      <c r="G29" s="59" t="s">
         <v>188</v>
       </c>
-      <c r="H29" s="53"/>
-      <c r="I29" s="58"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="55"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="13" t="s">
@@ -3767,11 +3767,11 @@
         <v>0.10416666666666667</v>
       </c>
       <c r="F30" s="16"/>
-      <c r="G30" s="57" t="s">
+      <c r="G30" s="59" t="s">
         <v>191</v>
       </c>
-      <c r="H30" s="53"/>
-      <c r="I30" s="58"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="55"/>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="13" t="s">
@@ -3786,9 +3786,9 @@
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="16"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="58"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="55"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="13" t="s">
@@ -3799,9 +3799,9 @@
       <c r="D32" s="16"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="54"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="58"/>
     </row>
     <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
@@ -3810,9 +3810,9 @@
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
       <c r="F33" s="16"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="55"/>
-      <c r="I33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="57"/>
+      <c r="I33" s="58"/>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="42" t="s">
@@ -3833,9 +3833,9 @@
       <c r="F34" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="G34" s="54"/>
-      <c r="H34" s="55"/>
-      <c r="I34" s="56"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="58"/>
     </row>
     <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="13" t="s">
@@ -3846,9 +3846,9 @@
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="54"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="58"/>
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="13" t="s">
@@ -3875,11 +3875,11 @@
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="54" t="s">
+      <c r="G37" s="56" t="s">
         <v>199</v>
       </c>
-      <c r="H37" s="55"/>
-      <c r="I37" s="56"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="58"/>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="13" t="s">
@@ -3894,11 +3894,11 @@
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="54" t="s">
+      <c r="G38" s="56" t="s">
         <v>201</v>
       </c>
-      <c r="H38" s="55"/>
-      <c r="I38" s="56"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="58"/>
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="13" t="s">
@@ -3913,11 +3913,11 @@
       </c>
       <c r="E39" s="12"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="54" t="s">
+      <c r="G39" s="56" t="s">
         <v>203</v>
       </c>
-      <c r="H39" s="55"/>
-      <c r="I39" s="56"/>
+      <c r="H39" s="57"/>
+      <c r="I39" s="58"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="13" t="s">
@@ -3932,9 +3932,9 @@
       </c>
       <c r="E40" s="12"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="54"/>
-      <c r="H40" s="55"/>
-      <c r="I40" s="56"/>
+      <c r="G40" s="56"/>
+      <c r="H40" s="57"/>
+      <c r="I40" s="58"/>
     </row>
     <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="16"/>
@@ -3943,9 +3943,9 @@
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
-      <c r="G41" s="54"/>
-      <c r="H41" s="55"/>
-      <c r="I41" s="56"/>
+      <c r="G41" s="56"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="58"/>
     </row>
     <row r="61" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="42"/>
@@ -3954,17 +3954,17 @@
       <c r="D61" s="42"/>
       <c r="E61" s="42"/>
       <c r="F61" s="42"/>
-      <c r="G61" s="54"/>
-      <c r="H61" s="55"/>
-      <c r="I61" s="56"/>
+      <c r="G61" s="56"/>
+      <c r="H61" s="57"/>
+      <c r="I61" s="58"/>
     </row>
     <row r="62" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="13"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
-      <c r="G62" s="54"/>
-      <c r="H62" s="55"/>
-      <c r="I62" s="56"/>
+      <c r="G62" s="56"/>
+      <c r="H62" s="57"/>
+      <c r="I62" s="58"/>
     </row>
     <row r="63" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="13"/>
@@ -3973,9 +3973,9 @@
       <c r="D63" s="2"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
-      <c r="G63" s="54"/>
-      <c r="H63" s="55"/>
-      <c r="I63" s="56"/>
+      <c r="G63" s="56"/>
+      <c r="H63" s="57"/>
+      <c r="I63" s="58"/>
     </row>
     <row r="64" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="13"/>
@@ -3984,47 +3984,12 @@
       <c r="D64" s="2"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
-      <c r="G64" s="54"/>
-      <c r="H64" s="55"/>
-      <c r="I64" s="56"/>
+      <c r="G64" s="56"/>
+      <c r="H64" s="57"/>
+      <c r="I64" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="G35:I35"/>
     <mergeCell ref="G63:I63"/>
     <mergeCell ref="G64:I64"/>
     <mergeCell ref="G37:I37"/>
@@ -4034,6 +3999,41 @@
     <mergeCell ref="G41:I41"/>
     <mergeCell ref="G61:I61"/>
     <mergeCell ref="G62:I62"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>